<commit_message>
Increase test coverage by adding example with incorrect path into variables when using `TemplateFormulaCell`
</commit_message>
<xml_diff>
--- a/packages/xlsx-renderer/tests/integration/data/Renderer017-TemplateFormula/expected.xlsx
+++ b/packages/xlsx-renderer/tests/integration/data/Renderer017-TemplateFormula/expected.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="5560" yWindow="1120" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Correct Formula" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Incorrect Formula" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Item</t>
   </si>
@@ -41,6 +42,9 @@
   </si>
   <si>
     <t>Custom formula:</t>
+  </si>
+  <si>
+    <t>Incorrect custom formula:</t>
   </si>
 </sst>
 </file>
@@ -79,7 +83,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,6 +93,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.7999816888943144"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.5999938962981048"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -105,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -113,6 +123,13 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -432,7 +449,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
@@ -523,4 +540,102 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>13.5</v>
+      </c>
+      <c r="C2">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>13.5</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3.5</v>
+      </c>
+      <c r="C4">
+        <v>12.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="8" ht="51" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7">
+        <f>MAX( Bundefined:Bundefined)</f>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>